<commit_message>
Compute counterfactual Law 27609 mobility for 2010-2020 period
</commit_message>
<xml_diff>
--- a/Excel_files_for_MISSAR/Social_security_data/Counterfactual_Law_26417_indexation.xlsx
+++ b/Excel_files_for_MISSAR/Social_security_data/Counterfactual_Law_26417_indexation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Fuentes salarios y recaudación" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,10 +16,6 @@
     <sheet name="Monto jubilación mínima" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Beneficios_SIPA" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
-  </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -1620,311 +1616,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="IPC"/>
-      <sheetName val="RIPTE"/>
-      <sheetName val="RIPTE e IPC"/>
-      <sheetName val="Rent autonomous"/>
-      <sheetName val="Payment autonomous"/>
-      <sheetName val="Minimum wage"/>
-      <sheetName val="PBU"/>
-      <sheetName val="Min pension"/>
-      <sheetName val="Max pension"/>
-      <sheetName val="Non taxable wage"/>
-      <sheetName val="globals_transposed_prosp"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="908">
-          <cell r="A908">
-            <v>2018</v>
-          </cell>
-        </row>
-        <row r="909">
-          <cell r="A909">
-            <v>2018</v>
-          </cell>
-        </row>
-        <row r="910">
-          <cell r="A910">
-            <v>2018</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Inflation and wages"/>
-      <sheetName val="Historical wage and tax income"/>
-      <sheetName val="Law 26.417 mobility computation"/>
-      <sheetName val="Población 2000-2040"/>
-      <sheetName val="Counterfactual Law 26.417 index"/>
-      <sheetName val="Law 26.417 index with retirees"/>
-      <sheetName val="Possible_semestral_mobility"/>
-      <sheetName val="Possible_quarterly_mobility"/>
-      <sheetName val="Pension mobility"/>
-      <sheetName val="Simulated_ANSES_contributions"/>
-      <sheetName val="Simulated_ANSES_contributions_2015"/>
-      <sheetName val="Fiscal ANSES income 2015 leg"/>
-      <sheetName val="Fiscal ANSES income 2020 leg"/>
-      <sheetName val="Pessimistic macro hypothesis"/>
-      <sheetName val="Pessimistic projection"/>
-      <sheetName val="Optimist macro hypothesis"/>
-      <sheetName val="Optimist projection"/>
-      <sheetName val="Central macro hypothesis"/>
-      <sheetName val="Central projection"/>
-      <sheetName val="Real wage scenarios"/>
-      <sheetName val="Real wage scenarios representat"/>
-      <sheetName val="Rent autonomous"/>
-      <sheetName val="Payment autonomous"/>
-      <sheetName val="Minimum wage"/>
-      <sheetName val="PBU"/>
-      <sheetName val="Min pension"/>
-      <sheetName val="Max pension"/>
-      <sheetName val="Non taxable wage_27430_Law"/>
-      <sheetName val="Non_taxable_wage_31_12_19_leg"/>
-      <sheetName val="Max_taxable_wage"/>
-      <sheetName val="globals_Macri_legislation"/>
-      <sheetName val="globals_2017_leg"/>
-      <sheetName val="globals_31_12_19_leg"/>
-      <sheetName val="globals_2020_legislation"/>
-      <sheetName val="globals_2020_leg_semestral"/>
-      <sheetName val="copy_to_csv_Macri_leg"/>
-      <sheetName val="copy_to_csv_2017_leg"/>
-      <sheetName val="copy_to_csv_31_12_19_leg"/>
-      <sheetName val="copy_to_csv_2020_leg"/>
-      <sheetName val="copy_to_csv_2020_leg_sem"/>
-      <sheetName val="RIPTE"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="923">
-          <cell r="N923">
-            <v>47834.32</v>
-          </cell>
-        </row>
-        <row r="924">
-          <cell r="N924">
-            <v>48591.6</v>
-          </cell>
-        </row>
-        <row r="925">
-          <cell r="N925">
-            <v>49574.33</v>
-          </cell>
-        </row>
-        <row r="926">
-          <cell r="N926">
-            <v>53070.21</v>
-          </cell>
-        </row>
-        <row r="927">
-          <cell r="N927">
-            <v>56386.47</v>
-          </cell>
-        </row>
-        <row r="928">
-          <cell r="N928">
-            <v>56872.86</v>
-          </cell>
-        </row>
-        <row r="929">
-          <cell r="N929">
-            <v>56955.63</v>
-          </cell>
-        </row>
-        <row r="930">
-          <cell r="N930">
-            <v>57057.9</v>
-          </cell>
-        </row>
-        <row r="931">
-          <cell r="N931">
-            <v>58361.93</v>
-          </cell>
-        </row>
-        <row r="932">
-          <cell r="N932">
-            <v>60440.53</v>
-          </cell>
-        </row>
-        <row r="933">
-          <cell r="N933">
-            <v>60767.23</v>
-          </cell>
-        </row>
-        <row r="934">
-          <cell r="N934">
-            <v>61909.95</v>
-          </cell>
-        </row>
-        <row r="935">
-          <cell r="N935">
-            <v>64756.23</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18">
-        <row r="293">
-          <cell r="A293">
-            <v>2018</v>
-          </cell>
-          <cell r="B293" t="str">
-            <v>Octubre</v>
-          </cell>
-        </row>
-        <row r="294">
-          <cell r="A294">
-            <v>2018</v>
-          </cell>
-          <cell r="B294" t="str">
-            <v>Noviembre</v>
-          </cell>
-        </row>
-        <row r="295">
-          <cell r="A295">
-            <v>2018</v>
-          </cell>
-          <cell r="B295" t="str">
-            <v>Diciembre</v>
-          </cell>
-        </row>
-        <row r="296">
-          <cell r="A296">
-            <v>2019</v>
-          </cell>
-          <cell r="B296" t="str">
-            <v>Enero</v>
-          </cell>
-        </row>
-        <row r="297">
-          <cell r="A297">
-            <v>2019</v>
-          </cell>
-          <cell r="B297" t="str">
-            <v>Febrero</v>
-          </cell>
-        </row>
-        <row r="298">
-          <cell r="A298">
-            <v>2019</v>
-          </cell>
-          <cell r="B298" t="str">
-            <v>Marzo</v>
-          </cell>
-        </row>
-        <row r="299">
-          <cell r="A299">
-            <v>2019</v>
-          </cell>
-          <cell r="B299" t="str">
-            <v>Abril</v>
-          </cell>
-        </row>
-        <row r="300">
-          <cell r="A300">
-            <v>2019</v>
-          </cell>
-          <cell r="B300" t="str">
-            <v>Mayo</v>
-          </cell>
-        </row>
-        <row r="301">
-          <cell r="A301">
-            <v>2019</v>
-          </cell>
-          <cell r="B301" t="str">
-            <v>Junio</v>
-          </cell>
-        </row>
-        <row r="302">
-          <cell r="A302">
-            <v>2019</v>
-          </cell>
-          <cell r="B302" t="str">
-            <v>Julio</v>
-          </cell>
-        </row>
-        <row r="303">
-          <cell r="A303">
-            <v>2019</v>
-          </cell>
-          <cell r="B303" t="str">
-            <v>Agosto</v>
-          </cell>
-        </row>
-        <row r="304">
-          <cell r="A304">
-            <v>2019</v>
-          </cell>
-          <cell r="B304" t="str">
-            <v>Septiembre</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -1932,12 +1623,12 @@
   </sheetPr>
   <dimension ref="A1:J319"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F297" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C299" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A297" activeCellId="0" sqref="A297"/>
-      <selection pane="bottomRight" activeCell="H310" activeCellId="0" sqref="H310"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A299" activeCellId="0" sqref="A299"/>
+      <selection pane="bottomRight" activeCell="D317" activeCellId="0" sqref="D317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.37109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7204,7 +6895,7 @@
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="4" t="n">
-        <f aca="false">'[1]RIPTE e IPC'!A908+1</f>
+        <f aca="false">A290+1</f>
         <v>2019</v>
       </c>
       <c r="B302" s="4" t="str">
@@ -7231,7 +6922,7 @@
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="22" t="n">
-        <f aca="false">'[1]RIPTE e IPC'!A909+1</f>
+        <f aca="false">A291+1</f>
         <v>2019</v>
       </c>
       <c r="B303" s="22" t="str">
@@ -7258,7 +6949,7 @@
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="6" t="n">
-        <f aca="false">'[1]RIPTE e IPC'!A910+1</f>
+        <f aca="false">A292+1</f>
         <v>2019</v>
       </c>
       <c r="B304" s="6" t="str">
@@ -7285,15 +6976,14 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="4" t="n">
-        <f aca="false">'[2]Central projection'!A293+1</f>
+        <f aca="false">A293+1</f>
         <v>2019</v>
       </c>
       <c r="B305" s="4" t="str">
-        <f aca="false">'[2]Central projection'!B293</f>
+        <f aca="false">B293</f>
         <v>Octubre</v>
       </c>
       <c r="C305" s="17" t="n">
-        <f aca="false">'[2]Inflation and wages'!N923</f>
         <v>47834.32</v>
       </c>
       <c r="D305" s="24" t="n">
@@ -7313,15 +7003,14 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="38" t="n">
-        <f aca="false">'[2]Central projection'!A294+1</f>
+        <f aca="false">A294+1</f>
         <v>2019</v>
       </c>
       <c r="B306" s="38" t="str">
-        <f aca="false">'[2]Central projection'!B294</f>
+        <f aca="false">B294</f>
         <v>Noviembre</v>
       </c>
       <c r="C306" s="23" t="n">
-        <f aca="false">'[2]Inflation and wages'!N924</f>
         <v>48591.6</v>
       </c>
       <c r="D306" s="24" t="n">
@@ -7341,15 +7030,14 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="6" t="n">
-        <f aca="false">'[2]Central projection'!A295+1</f>
+        <f aca="false">A295+1</f>
         <v>2019</v>
       </c>
       <c r="B307" s="6" t="str">
-        <f aca="false">'[2]Central projection'!B295</f>
+        <f aca="false">B295</f>
         <v>Diciembre</v>
       </c>
       <c r="C307" s="21" t="n">
-        <f aca="false">'[2]Inflation and wages'!N925</f>
         <v>49574.33</v>
       </c>
       <c r="D307" s="24" t="n">
@@ -7369,15 +7057,14 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="4" t="n">
-        <f aca="false">'[2]Central projection'!A296+1</f>
+        <f aca="false">A296+1</f>
         <v>2020</v>
       </c>
       <c r="B308" s="4" t="str">
-        <f aca="false">'[2]Central projection'!B296</f>
+        <f aca="false">B296</f>
         <v>Enero</v>
       </c>
       <c r="C308" s="17" t="n">
-        <f aca="false">'[2]Inflation and wages'!N926</f>
         <v>53070.21</v>
       </c>
       <c r="D308" s="24" t="n">
@@ -7402,15 +7089,14 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="38" t="n">
-        <f aca="false">'[2]Central projection'!A297+1</f>
+        <f aca="false">A297+1</f>
         <v>2020</v>
       </c>
       <c r="B309" s="38" t="str">
-        <f aca="false">'[2]Central projection'!B297</f>
+        <f aca="false">B297</f>
         <v>Febrero</v>
       </c>
       <c r="C309" s="23" t="n">
-        <f aca="false">'[2]Inflation and wages'!N927</f>
         <v>56386.47</v>
       </c>
       <c r="D309" s="39" t="n">
@@ -7432,15 +7118,14 @@
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="6" t="n">
-        <f aca="false">'[2]Central projection'!A298+1</f>
+        <f aca="false">A298+1</f>
         <v>2020</v>
       </c>
       <c r="B310" s="6" t="str">
-        <f aca="false">'[2]Central projection'!B298</f>
+        <f aca="false">B298</f>
         <v>Marzo</v>
       </c>
       <c r="C310" s="21" t="n">
-        <f aca="false">'[2]Inflation and wages'!N928</f>
         <v>56872.86</v>
       </c>
       <c r="D310" s="39" t="n">
@@ -7462,15 +7147,14 @@
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="4" t="n">
-        <f aca="false">'[2]Central projection'!A299+1</f>
+        <f aca="false">A299+1</f>
         <v>2020</v>
       </c>
       <c r="B311" s="4" t="str">
-        <f aca="false">'[2]Central projection'!B299</f>
+        <f aca="false">B299</f>
         <v>Abril</v>
       </c>
       <c r="C311" s="17" t="n">
-        <f aca="false">'[2]Inflation and wages'!N929</f>
         <v>56955.63</v>
       </c>
       <c r="D311" s="40" t="n">
@@ -7492,15 +7176,14 @@
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="38" t="n">
-        <f aca="false">'[2]Central projection'!A300+1</f>
+        <f aca="false">A300+1</f>
         <v>2020</v>
       </c>
       <c r="B312" s="38" t="str">
-        <f aca="false">'[2]Central projection'!B300</f>
+        <f aca="false">B300</f>
         <v>Mayo</v>
       </c>
       <c r="C312" s="23" t="n">
-        <f aca="false">'[2]Inflation and wages'!N930</f>
         <v>57057.9</v>
       </c>
       <c r="D312" s="39" t="n">
@@ -7522,15 +7205,14 @@
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="6" t="n">
-        <f aca="false">'[2]Central projection'!A301+1</f>
+        <f aca="false">A301+1</f>
         <v>2020</v>
       </c>
       <c r="B313" s="6" t="str">
-        <f aca="false">'[2]Central projection'!B301</f>
+        <f aca="false">B301</f>
         <v>Junio</v>
       </c>
       <c r="C313" s="21" t="n">
-        <f aca="false">'[2]Inflation and wages'!N931</f>
         <v>58361.93</v>
       </c>
       <c r="D313" s="39" t="n">
@@ -7552,15 +7234,14 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="4" t="n">
-        <f aca="false">'[2]Central projection'!A302+1</f>
+        <f aca="false">A302+1</f>
         <v>2020</v>
       </c>
       <c r="B314" s="4" t="str">
-        <f aca="false">'[2]Central projection'!B302</f>
+        <f aca="false">B302</f>
         <v>Julio</v>
       </c>
       <c r="C314" s="41" t="n">
-        <f aca="false">'[2]Inflation and wages'!N932</f>
         <v>60440.53</v>
       </c>
       <c r="D314" s="39" t="n">
@@ -7586,15 +7267,14 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="38" t="n">
-        <f aca="false">'[2]Central projection'!A303+1</f>
+        <f aca="false">A303+1</f>
         <v>2020</v>
       </c>
       <c r="B315" s="38" t="str">
-        <f aca="false">'[2]Central projection'!B303</f>
+        <f aca="false">B303</f>
         <v>Agosto</v>
       </c>
       <c r="C315" s="23" t="n">
-        <f aca="false">'[2]Inflation and wages'!N933</f>
         <v>60767.23</v>
       </c>
       <c r="D315" s="39" t="n">
@@ -7616,15 +7296,14 @@
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="6" t="n">
-        <f aca="false">'[2]Central projection'!A304+1</f>
+        <f aca="false">A304+1</f>
         <v>2020</v>
       </c>
       <c r="B316" s="6" t="str">
-        <f aca="false">'[2]Central projection'!B304</f>
+        <f aca="false">B304</f>
         <v>Septiembre</v>
       </c>
       <c r="C316" s="21" t="n">
-        <f aca="false">'[2]Inflation and wages'!N934</f>
         <v>61909.95</v>
       </c>
       <c r="D316" s="44" t="n">
@@ -7646,15 +7325,14 @@
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="4" t="n">
-        <f aca="false">'Fuentes salarios y recaudación'!A305+1</f>
+        <f aca="false">A305+1</f>
         <v>2020</v>
       </c>
       <c r="B317" s="4" t="str">
-        <f aca="false">'Fuentes salarios y recaudación'!B305</f>
+        <f aca="false">B305</f>
         <v>Octubre</v>
       </c>
       <c r="C317" s="17" t="n">
-        <f aca="false">'[2]Inflation and wages'!N935</f>
         <v>64756.23</v>
       </c>
       <c r="D317" s="45" t="n">
@@ -7672,11 +7350,11 @@
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="38" t="n">
-        <f aca="false">'Fuentes salarios y recaudación'!A306+1</f>
+        <f aca="false">A306+1</f>
         <v>2020</v>
       </c>
       <c r="B318" s="38" t="str">
-        <f aca="false">'Fuentes salarios y recaudación'!B306</f>
+        <f aca="false">B306</f>
         <v>Noviembre</v>
       </c>
       <c r="C318" s="23"/>
@@ -7692,11 +7370,11 @@
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="6" t="n">
-        <f aca="false">'Fuentes salarios y recaudación'!A307+1</f>
+        <f aca="false">A307+1</f>
         <v>2020</v>
       </c>
       <c r="B319" s="6" t="str">
-        <f aca="false">'Fuentes salarios y recaudación'!B307</f>
+        <f aca="false">B307</f>
         <v>Diciembre</v>
       </c>
       <c r="C319" s="21"/>
@@ -7728,7 +7406,7 @@
   </sheetPr>
   <dimension ref="B2:L141"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L135" activeCellId="0" sqref="L135"/>
     </sheetView>
   </sheetViews>

</xml_diff>